<commit_message>
Solved issue w/ persistence of tasks in path
</commit_message>
<xml_diff>
--- a/src/main/resources/dataloader_empty_long.xlsx
+++ b/src/main/resources/dataloader_empty_long.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
@@ -15,306 +15,276 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
-  <si>
-    <t>_taskShort1</t>
-  </si>
-  <si>
-    <t>_taskShort2</t>
-  </si>
-  <si>
-    <t>_taskShort3</t>
-  </si>
-  <si>
-    <t>_taskShort4</t>
-  </si>
-  <si>
-    <t>_taskShort5</t>
-  </si>
-  <si>
-    <t>_taskShort6</t>
-  </si>
-  <si>
-    <t>_taskShort7</t>
-  </si>
-  <si>
-    <t>_taskShort8</t>
-  </si>
-  <si>
-    <t>_taskShort9</t>
-  </si>
-  <si>
-    <t>_taskShort10</t>
-  </si>
-  <si>
-    <t>_taskShort11</t>
-  </si>
-  <si>
-    <t>_taskShort12</t>
-  </si>
-  <si>
-    <t>_taskShort13</t>
-  </si>
-  <si>
-    <t>_taskShort14</t>
-  </si>
-  <si>
-    <t>_taskShort15</t>
-  </si>
-  <si>
-    <t>_taskShort16</t>
-  </si>
-  <si>
-    <t>_taskShort17</t>
-  </si>
-  <si>
-    <t>_taskShort18</t>
-  </si>
-  <si>
-    <t>_taskShort19</t>
-  </si>
-  <si>
-    <t>_taskShort20</t>
-  </si>
-  <si>
-    <t>_taskShort21</t>
-  </si>
-  <si>
-    <t>_taskShort22</t>
-  </si>
-  <si>
-    <t>_taskShort23</t>
-  </si>
-  <si>
-    <t>_taskShort24</t>
-  </si>
-  <si>
-    <t>_taskShort25</t>
-  </si>
-  <si>
-    <t>_taskShort26</t>
-  </si>
-  <si>
-    <t>_taskShort27</t>
-  </si>
-  <si>
-    <t>_taskShort28</t>
-  </si>
-  <si>
-    <t>_taskLong1</t>
-  </si>
-  <si>
-    <t>_taskLong2</t>
-  </si>
-  <si>
-    <t>_taskLong4</t>
-  </si>
-  <si>
-    <t>_taskLong5</t>
-  </si>
-  <si>
-    <t>_taskLong7</t>
-  </si>
-  <si>
-    <t>_taskLong8</t>
-  </si>
-  <si>
-    <t>_taskLong9</t>
-  </si>
-  <si>
-    <t>_taskLong11</t>
-  </si>
-  <si>
-    <t>_taskLong12</t>
-  </si>
-  <si>
-    <t>_taskLong13</t>
-  </si>
-  <si>
-    <t>_taskLong14</t>
-  </si>
-  <si>
-    <t>_taskLong15</t>
-  </si>
-  <si>
-    <t>_taskLong16</t>
-  </si>
-  <si>
-    <t>_taskLong17</t>
-  </si>
-  <si>
-    <t>_taskLong19</t>
-  </si>
-  <si>
-    <t>_taskLong20</t>
-  </si>
-  <si>
-    <t>_taskLong21</t>
-  </si>
-  <si>
-    <t>_taskLong22</t>
-  </si>
-  <si>
-    <t>_taskLong23</t>
-  </si>
-  <si>
-    <t>_taskLong25</t>
-  </si>
-  <si>
-    <t>_taskLong26</t>
-  </si>
-  <si>
-    <t>_taskLong28</t>
-  </si>
-  <si>
-    <t>_PathShort1</t>
-  </si>
-  <si>
-    <t>_PathShort2</t>
-  </si>
-  <si>
-    <t>_PathShort3</t>
-  </si>
-  <si>
-    <t>_PathShort4</t>
-  </si>
-  <si>
-    <t>_PathShort5</t>
-  </si>
-  <si>
-    <t>_PathShort6</t>
-  </si>
-  <si>
-    <t>_PathLong6</t>
-  </si>
-  <si>
-    <t>_taskShort29</t>
-  </si>
-  <si>
-    <t>_taskShort30</t>
-  </si>
-  <si>
-    <t>_taskLong29</t>
-  </si>
-  <si>
-    <t>_taskLong30</t>
-  </si>
-  <si>
-    <t>_PathName55</t>
-  </si>
-  <si>
-    <t>_PathName56</t>
-  </si>
-  <si>
-    <t>_PathName57</t>
-  </si>
-  <si>
-    <t>_PathName58</t>
-  </si>
-  <si>
-    <t>_PathName59</t>
-  </si>
-  <si>
-    <t>_PathName60</t>
-  </si>
-  <si>
-    <t>_taskName55</t>
-  </si>
-  <si>
-    <t>_taskName56</t>
-  </si>
-  <si>
-    <t>_taskName57</t>
-  </si>
-  <si>
-    <t>_taskName58</t>
-  </si>
-  <si>
-    <t>_taskName59</t>
-  </si>
-  <si>
-    <t>_taskName60</t>
-  </si>
-  <si>
-    <t>_taskName61</t>
-  </si>
-  <si>
-    <t>_taskName62</t>
-  </si>
-  <si>
-    <t>_taskName63</t>
-  </si>
-  <si>
-    <t>_taskName64</t>
-  </si>
-  <si>
-    <t>_taskName65</t>
-  </si>
-  <si>
-    <t>_taskName66</t>
-  </si>
-  <si>
-    <t>_taskName67</t>
-  </si>
-  <si>
-    <t>_taskName68</t>
-  </si>
-  <si>
-    <t>_taskName69</t>
-  </si>
-  <si>
-    <t>_taskName70</t>
-  </si>
-  <si>
-    <t>_taskName71</t>
-  </si>
-  <si>
-    <t>_taskName72</t>
-  </si>
-  <si>
-    <t>_taskName73</t>
-  </si>
-  <si>
-    <t>_taskName74</t>
-  </si>
-  <si>
-    <t>_taskName75</t>
-  </si>
-  <si>
-    <t>_taskName76</t>
-  </si>
-  <si>
-    <t>_taskName77</t>
-  </si>
-  <si>
-    <t>_taskName78</t>
-  </si>
-  <si>
-    <t>_taskName79</t>
-  </si>
-  <si>
-    <t>_taskName80</t>
-  </si>
-  <si>
-    <t>_taskName81</t>
-  </si>
-  <si>
-    <t>_taskName82</t>
-  </si>
-  <si>
-    <t>_taskName83</t>
-  </si>
-  <si>
-    <t>_taskName84</t>
-  </si>
-  <si>
-    <t>_PathLong27</t>
-  </si>
-  <si>
-    <t>_PathLong37</t>
-  </si>
-  <si>
-    <t>_PathLong57</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+  <si>
+    <t>?PathName55</t>
+  </si>
+  <si>
+    <t>?PathName56</t>
+  </si>
+  <si>
+    <t>?PathName57</t>
+  </si>
+  <si>
+    <t>?PathName58</t>
+  </si>
+  <si>
+    <t>?PathName59</t>
+  </si>
+  <si>
+    <t>?PathName60</t>
+  </si>
+  <si>
+    <t>?PathShort1</t>
+  </si>
+  <si>
+    <t>?PathShort2</t>
+  </si>
+  <si>
+    <t>?PathShort3</t>
+  </si>
+  <si>
+    <t>?PathShort4</t>
+  </si>
+  <si>
+    <t>?PathShort5</t>
+  </si>
+  <si>
+    <t>?PathShort6</t>
+  </si>
+  <si>
+    <t>?PathLong27</t>
+  </si>
+  <si>
+    <t>?PathLong37</t>
+  </si>
+  <si>
+    <t>?PathLong57</t>
+  </si>
+  <si>
+    <t>?PathLong6</t>
+  </si>
+  <si>
+    <t>?taskName55</t>
+  </si>
+  <si>
+    <t>?taskName56</t>
+  </si>
+  <si>
+    <t>?taskName57</t>
+  </si>
+  <si>
+    <t>?taskName58</t>
+  </si>
+  <si>
+    <t>?taskName59</t>
+  </si>
+  <si>
+    <t>?taskName60</t>
+  </si>
+  <si>
+    <t>?taskName61</t>
+  </si>
+  <si>
+    <t>?taskName62</t>
+  </si>
+  <si>
+    <t>?taskName63</t>
+  </si>
+  <si>
+    <t>?taskName64</t>
+  </si>
+  <si>
+    <t>?taskName65</t>
+  </si>
+  <si>
+    <t>?taskName66</t>
+  </si>
+  <si>
+    <t>?taskName67</t>
+  </si>
+  <si>
+    <t>?taskName68</t>
+  </si>
+  <si>
+    <t>?taskName69</t>
+  </si>
+  <si>
+    <t>?taskName70</t>
+  </si>
+  <si>
+    <t>?taskName71</t>
+  </si>
+  <si>
+    <t>?taskName72</t>
+  </si>
+  <si>
+    <t>?taskName73</t>
+  </si>
+  <si>
+    <t>?taskName74</t>
+  </si>
+  <si>
+    <t>?taskName75</t>
+  </si>
+  <si>
+    <t>?taskName76</t>
+  </si>
+  <si>
+    <t>?taskName77</t>
+  </si>
+  <si>
+    <t>?taskName78</t>
+  </si>
+  <si>
+    <t>?taskName79</t>
+  </si>
+  <si>
+    <t>?taskName80</t>
+  </si>
+  <si>
+    <t>?taskName81</t>
+  </si>
+  <si>
+    <t>?taskName82</t>
+  </si>
+  <si>
+    <t>?taskName83</t>
+  </si>
+  <si>
+    <t>?taskName84</t>
+  </si>
+  <si>
+    <t>?taskShort1</t>
+  </si>
+  <si>
+    <t>?taskShort2</t>
+  </si>
+  <si>
+    <t>?taskShort3</t>
+  </si>
+  <si>
+    <t>?taskShort4</t>
+  </si>
+  <si>
+    <t>?taskShort5</t>
+  </si>
+  <si>
+    <t>?taskShort6</t>
+  </si>
+  <si>
+    <t>?taskShort7</t>
+  </si>
+  <si>
+    <t>?taskShort8</t>
+  </si>
+  <si>
+    <t>?taskShort9</t>
+  </si>
+  <si>
+    <t>?taskShort10</t>
+  </si>
+  <si>
+    <t>?taskShort11</t>
+  </si>
+  <si>
+    <t>?taskShort12</t>
+  </si>
+  <si>
+    <t>?taskShort13</t>
+  </si>
+  <si>
+    <t>?taskShort14</t>
+  </si>
+  <si>
+    <t>?taskShort15</t>
+  </si>
+  <si>
+    <t>?taskShort16</t>
+  </si>
+  <si>
+    <t>?taskShort17</t>
+  </si>
+  <si>
+    <t>?taskShort18</t>
+  </si>
+  <si>
+    <t>?taskShort19</t>
+  </si>
+  <si>
+    <t>?taskShort20</t>
+  </si>
+  <si>
+    <t>?taskShort21</t>
+  </si>
+  <si>
+    <t>?taskShort22</t>
+  </si>
+  <si>
+    <t>?taskShort23</t>
+  </si>
+  <si>
+    <t>?taskShort24</t>
+  </si>
+  <si>
+    <t>?taskShort25</t>
+  </si>
+  <si>
+    <t>?taskShort26</t>
+  </si>
+  <si>
+    <t>?taskShort27</t>
+  </si>
+  <si>
+    <t>?taskShort28</t>
+  </si>
+  <si>
+    <t>?taskShort29</t>
+  </si>
+  <si>
+    <t>?taskShort30</t>
+  </si>
+  <si>
+    <t>?taskLong1</t>
+  </si>
+  <si>
+    <t>?taskLong2</t>
+  </si>
+  <si>
+    <t>?taskLong4</t>
+  </si>
+  <si>
+    <t>?taskLong5</t>
+  </si>
+  <si>
+    <t>?taskLong7</t>
+  </si>
+  <si>
+    <t>?taskLong8</t>
+  </si>
+  <si>
+    <t>?taskLong9</t>
+  </si>
+  <si>
+    <t>?taskLong11</t>
+  </si>
+  <si>
+    <t>?taskLong12</t>
+  </si>
+  <si>
+    <t>?taskLong13</t>
+  </si>
+  <si>
+    <t>?taskLong14</t>
+  </si>
+  <si>
+    <t>?taskLong15</t>
+  </si>
+  <si>
+    <t>?taskLong16</t>
+  </si>
+  <si>
+    <t>?taskLong17</t>
   </si>
 </sst>
 </file>
@@ -655,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,314 +637,284 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -986,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,62 +937,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>